<commit_message>
feat: confirando excesoes e aplicando navegacao para solicitar emprestimos
</commit_message>
<xml_diff>
--- a/Data/Input/Loan Quotes.xlsx
+++ b/Data/Input/Loan Quotes.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suzano-my.sharepoint.com/personal/julianobs_suzano_com_br/Documents/Area Dev/GitHub/UiPath/RoboPedidoDeEmprestimos/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_A73A42D88E7424E5259C5B2F92C3664882F1307B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8639455-CFBA-4891-B37E-3F885D9F82A5}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_A73A42D88E7424E5259C5B2F92C3664882F1307B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F5A63D4-B10D-4F5C-B13B-39FD6D6114DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,31 @@
     <sheet name="Loan Quotes" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+  <si>
+    <t>LoanName</t>
+  </si>
   <si>
     <t>LoanEmail</t>
   </si>
@@ -52,7 +66,28 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Michael Turner</t>
+  </si>
+  <si>
     <t>uipath@gmail.com</t>
+  </si>
+  <si>
+    <t>Sophie Bennett</t>
+  </si>
+  <si>
+    <t>Ethan Collins</t>
+  </si>
+  <si>
+    <t>Laura Mitchell</t>
+  </si>
+  <si>
+    <t>Daniel Foster</t>
+  </si>
+  <si>
+    <t>Emma Rogers</t>
+  </si>
+  <si>
+    <t>Henry Sullivan</t>
   </si>
   <si>
     <t>Sorry, at this time you have not been approved for a loan.</t>
@@ -156,14 +191,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +232,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +338,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,24 +488,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="20.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="52.85546875" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="20.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="52.85546875" style="3" customWidth="1"/>
+    <col min="9" max="10" width="12.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -499,135 +531,167 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
         <v>120000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>30000</v>
-      </c>
       <c r="E2" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F2" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
         <v>15000</v>
       </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
       <c r="D3" s="2">
-        <v>30000</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="2">
         <v>35</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
         <v>4000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
-        <v>30000</v>
-      </c>
       <c r="E4" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F4" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
         <v>7500</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
-        <v>30000</v>
-      </c>
       <c r="E5" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F5" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
         <v>2000</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>30000</v>
-      </c>
       <c r="E6" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F6" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
         <v>7500</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
-        <v>30000</v>
-      </c>
       <c r="E7" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F7" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
         <v>7500</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="2">
-        <v>30000</v>
-      </c>
       <c r="E8" s="2">
+        <v>30000</v>
+      </c>
+      <c r="F8" s="2">
         <v>16</v>
       </c>
-      <c r="F8"/>
       <c r="G8"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -656,34 +720,34 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>120000</v>
@@ -698,15 +762,15 @@
         <v>35</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>15000</v>
@@ -721,13 +785,13 @@
         <v>35</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,15 +808,15 @@
         <v>35</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>7500</v>
@@ -767,18 +831,18 @@
         <v>65</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>2000</v>
@@ -793,18 +857,18 @@
         <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>7500</v>
@@ -819,18 +883,18 @@
         <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>7500</v>
@@ -845,10 +909,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>